<commit_message>
updates in the jupyter notebook
</commit_message>
<xml_diff>
--- a/Data challenges_summeries_climathon_HP2.xlsx
+++ b/Data challenges_summeries_climathon_HP2.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/holgerprang/Documents/git/ckicscrape/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7018DFA1-6DFF-6843-85A2-A56D7C13AD36}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A49A6C-BF31-D543-9525-D1945F608B9E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19700"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summeries" sheetId="1" r:id="rId1"/>
@@ -3985,7 +3985,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -4826,11 +4826,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
-      <selection activeCell="G69" sqref="G69"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5394,7 +5394,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="144" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>153</v>
       </c>
@@ -5539,7 +5539,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="96" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>195</v>
       </c>
@@ -5568,7 +5568,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>203</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>212</v>
       </c>
@@ -5974,7 +5974,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>311</v>
       </c>
@@ -6003,7 +6003,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>319</v>
       </c>
@@ -6032,7 +6032,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>326</v>
       </c>
@@ -6061,7 +6061,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>333</v>
       </c>
@@ -6090,7 +6090,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="96" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>340</v>
       </c>
@@ -6148,7 +6148,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="96" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>355</v>
       </c>
@@ -6319,7 +6319,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="128" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>400</v>
       </c>
@@ -6577,7 +6577,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>468</v>
       </c>
@@ -6780,7 +6780,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" ht="128" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>521</v>
       </c>
@@ -7328,7 +7328,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" ht="144" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>667</v>
       </c>
@@ -7357,7 +7357,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" ht="128" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>674</v>
       </c>
@@ -7386,7 +7386,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" ht="144" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>681</v>
       </c>
@@ -7705,7 +7705,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" ht="96" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>763</v>
       </c>

</xml_diff>